<commit_message>
Create first draft for combat module
</commit_message>
<xml_diff>
--- a/design-documents/progression-tables.xlsx
+++ b/design-documents/progression-tables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal-web-projects\kill-the-dragon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal-web-projects\kill-the-dragon\design-documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -59,18 +59,6 @@
     <t>mob</t>
   </si>
   <si>
-    <t>Wolf 1</t>
-  </si>
-  <si>
-    <t>Wolf 2</t>
-  </si>
-  <si>
-    <t>Sorcerer</t>
-  </si>
-  <si>
-    <t>Warrior</t>
-  </si>
-  <si>
     <t>weak</t>
   </si>
   <si>
@@ -110,18 +98,6 @@
     <t>water</t>
   </si>
   <si>
-    <t>Sorcerer 1</t>
-  </si>
-  <si>
-    <t>Sorcerer2</t>
-  </si>
-  <si>
-    <t>Warrior 1</t>
-  </si>
-  <si>
-    <t>Warrior 2</t>
-  </si>
-  <si>
     <t>Boss</t>
   </si>
   <si>
@@ -132,6 +108,30 @@
   </si>
   <si>
     <t>gold</t>
+  </si>
+  <si>
+    <t>Ella Jarvis</t>
+  </si>
+  <si>
+    <t>Maggie Ortega</t>
+  </si>
+  <si>
+    <t>Puck Yaztromo</t>
+  </si>
+  <si>
+    <t>Ron Doom</t>
+  </si>
+  <si>
+    <t>Danica Lacroix</t>
+  </si>
+  <si>
+    <t>Isobel Flowright</t>
+  </si>
+  <si>
+    <t>Wolf I</t>
+  </si>
+  <si>
+    <t>Wolf II</t>
   </si>
 </sst>
 </file>
@@ -903,12 +903,12 @@
   <dimension ref="B1:W18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="13" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -944,12 +944,12 @@
         <v>8</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>1</v>
@@ -979,7 +979,7 @@
     </row>
     <row r="4" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="29" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C4" s="9">
         <v>1</v>
@@ -1009,7 +1009,7 @@
         <v>1</v>
       </c>
       <c r="M4" s="29" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="N4" s="41">
         <v>20</v>
@@ -1033,7 +1033,7 @@
         <v>0</v>
       </c>
       <c r="U4" s="44" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="V4" s="8" t="s">
         <v>9</v>
@@ -1041,7 +1041,7 @@
     </row>
     <row r="5" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="27" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C5" s="17">
         <v>2</v>
@@ -1071,7 +1071,7 @@
         <v>1</v>
       </c>
       <c r="M5" s="27" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="N5" s="18">
         <v>20</v>
@@ -1095,10 +1095,10 @@
         <v>0</v>
       </c>
       <c r="U5" s="33" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="V5" s="24" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="W5" s="25">
         <v>40</v>
@@ -1106,7 +1106,7 @@
     </row>
     <row r="6" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="28" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C6" s="13">
         <v>3</v>
@@ -1136,7 +1136,7 @@
         <v>2</v>
       </c>
       <c r="M6" s="28" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="N6" s="14">
         <v>50</v>
@@ -1160,10 +1160,10 @@
         <v>0.05</v>
       </c>
       <c r="U6" s="34" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="V6" s="50" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="W6" s="6">
         <v>20</v>
@@ -1171,7 +1171,7 @@
     </row>
     <row r="7" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="27" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C7" s="17">
         <v>4</v>
@@ -1201,7 +1201,7 @@
         <v>2</v>
       </c>
       <c r="M7" s="30" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="N7" s="36">
         <v>50</v>
@@ -1225,12 +1225,12 @@
         <v>0</v>
       </c>
       <c r="U7" s="39" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="51" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C8" s="21">
         <v>5</v>
@@ -1273,7 +1273,7 @@
         <v>3</v>
       </c>
       <c r="M10" s="29" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N10" s="41">
         <v>80</v>
@@ -1296,19 +1296,19 @@
       <c r="T10" s="43">
         <v>0.1</v>
       </c>
-      <c r="U10" s="44" t="s">
-        <v>17</v>
+      <c r="U10" s="34" t="s">
+        <v>22</v>
       </c>
       <c r="V10" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L11" s="32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M11" s="27" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="N11" s="18">
         <v>80</v>
@@ -1331,11 +1331,11 @@
       <c r="T11" s="20">
         <v>0.1</v>
       </c>
-      <c r="U11" s="33" t="s">
-        <v>18</v>
+      <c r="U11" s="34" t="s">
+        <v>22</v>
       </c>
       <c r="V11" s="22" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="W11" s="6">
         <v>100</v>
@@ -1343,10 +1343,10 @@
     </row>
     <row r="12" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L12" s="31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M12" s="28" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="N12" s="14">
         <v>100</v>
@@ -1369,11 +1369,11 @@
       <c r="T12" s="16">
         <v>0</v>
       </c>
-      <c r="U12" s="34" t="s">
-        <v>26</v>
+      <c r="U12" s="39" t="s">
+        <v>23</v>
       </c>
       <c r="V12" s="50" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="W12" s="23">
         <v>40</v>
@@ -1408,7 +1408,7 @@
         <v>0</v>
       </c>
       <c r="U13" s="39" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.25">
@@ -1422,7 +1422,7 @@
         <v>5</v>
       </c>
       <c r="M16" s="46" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="N16" s="47">
         <v>700</v>
@@ -1446,27 +1446,27 @@
         <v>0.2</v>
       </c>
       <c r="U16" s="49" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="V16" s="8" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="12:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L17" s="3"/>
       <c r="V17" s="24" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="W17" s="25" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="12:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="V18" s="50" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="W18" s="6" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>